<commit_message>
add PL and FR translations
</commit_message>
<xml_diff>
--- a/tools/gdpr/gdpr-checklist.xlsx
+++ b/tools/gdpr/gdpr-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/gdpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5709A82B-3B56-AC47-9A73-03B62F24233C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02237E5-0BF9-2C44-BB6B-73A3F1642CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" xr2:uid="{D548BFD9-24AA-6740-B2D6-47677657AB26}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{D548BFD9-24AA-6740-B2D6-47677657AB26}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
   <si>
     <t>Conduct an information audit to determine what information you process and who has access to it.</t>
   </si>
@@ -275,6 +275,310 @@
   </si>
   <si>
     <t>requirements</t>
+  </si>
+  <si>
+    <t>Podstawy prawne i przejrzystość</t>
+  </si>
+  <si>
+    <t>Przeprowadź audyt informacji, aby określić, jakie informacje przetwarzasz i kto ma do nich dostęp.</t>
+  </si>
+  <si>
+    <t>Uzyskaj uzasadnienie prawne dla swoich działań przetwarzania danych.</t>
+  </si>
+  <si>
+    <t>Przetwarzanie danych jest nielegalne zgodnie z RODO, jeśli nie możesz go uzasadnić jednym z sześciu warunków wymienionych w art. 6. Są też inne przepisy dotyczące dzieci i specjalnych kategorii danych osobowych w art. 7-11. Przejrzyj te przepisy, wybierz prawidłową podstawę prawną przetwarzania i udokumentuj swoje uzasadnienie. Pamiętaj, że jeśli wybierzesz "zgodę" jako podstawę prawną, ciążą na Tobie dodatkowe obowiązki, w tym zapewnienie osobom, których dane dotyczą, ciągłej możliwości wycofania zgody. Jeśli twoją podstawą prawną są "uzasadnione interesy", musisz być w stanie wykazać, że przeprowadziłeś ocenę wpływu na prywatność.</t>
+  </si>
+  <si>
+    <t>Podaj jasne informacje o przetwarzaniu danych i uzasadnieniu prawnym w polityce prywatności.</t>
+  </si>
+  <si>
+    <t>Musisz poinformować osoby, że zbierasz ich dane i dlaczego (Art. 12 RODO). Powinieneś wyjaśnić, jak dane są przetwarzane, kto ma do nich dostęp i jak je zabezpieczasz. Informacje te powinny być zawarte w twojej polityce prywatności i dostarczone osobom, których dane dotyczą w momencie ich zbierania. Muszą być one przedstawione "w sposób zwięzły, przejrzysty, zrozumiały i łatwo dostępny, przy użyciu jasnego i prostego języka, szczególnie jeśli informacje są skierowane specjalnie do dziecka."</t>
+  </si>
+  <si>
+    <t>Bezpieczeństwo danych</t>
+  </si>
+  <si>
+    <t>Uwzględniaj ochronę danych przez cały czas, od momentu rozpoczęcia tworzenia produktu po każdorazowe przetwarzanie danych.</t>
+  </si>
+  <si>
+    <t>Szyfruj, pseudonimizuj lub anonimizuj dane osobowe tam, gdzie to możliwe.</t>
+  </si>
+  <si>
+    <t>Utwórz wewnętrzną politykę bezpieczeństwa dla członków swojego zespołu i zwiększaj świadomość ochrony danych.</t>
+  </si>
+  <si>
+    <t>Wiedz, kiedy przeprowadzić ocenę wpływu na ochronę danych i mieć procedurę umożliwiającą jej przeprowadzenie.</t>
+  </si>
+  <si>
+    <t>Posiadac procedurę powiadamiania władz i osób, których dane dotyczą, w przypadku naruszenia bezpieczeństwa danych.</t>
+  </si>
+  <si>
+    <t>Odpowiedzialność i zarządzanie</t>
+  </si>
+  <si>
+    <t>Wyznacz osobę odpowiedzialną za zapewnienie zgodności z RODO w całej organizacji.</t>
+  </si>
+  <si>
+    <t>Obejmuje to wszelkie usługi stron trzecich, które przetwarzają dane osobowe Twoich osób, w tym oprogramowanie analityczne, usługi e-mail, serwery w chmurze itp. Większość usług ma standardową umowę o przetwarzanie danych dostępną na swoich stronach internetowych do przeglądu. Określają one prawa i obowiązki każdej ze stron zgodnie z RODO. Powinieneś korzystać tylko z wiarygodnych stron trzecich, które mogą zagwarantować wystarczającą ochronę danych.</t>
+  </si>
+  <si>
+    <t>Rób wszystko, co w Twojej mocy, aby dane były aktualne, wprowadzając proces kontroli jakości danych, i umożliwiaj swoim klientom wgląd (Artykuł 15) i aktualizację swoich danych osobowych w celu zachowania ich dokładności i kompletności. Upewnij się, że możesz zweryfikować tożsamość osoby składającej wniosek. Powinieneś być w stanie zrealizować wnioski zgodnie z Artykułem 16 w ciągu miesiąca.</t>
+  </si>
+  <si>
+    <t>Osoby mają prawo żądać usunięcia wszystkich swoich danych osobowych, a Ty musisz spełnić ich żądanie w ciągu miesiąca. Istnieje pięć powodów, dla których możesz odmówić wniosku, takich jak korzystanie z wolności wypowiedzi czy wypełnianie obowiązku prawnego. Musisz także spróbować zweryfikować tożsamość osoby składającej wniosek.</t>
+  </si>
+  <si>
+    <t>Prawa prywatności,</t>
+  </si>
+  <si>
+    <t>Twoje osoby, których dane dotyczą, mogą zażądać ograniczenia lub zaprzestania przetwarzania ich danych (Artykuł 18), jeśli zachodzą pewne podstawy, głównie w przypadku sporu co do zgodności z prawem przetwarzania lub dokładności danych. Musisz spełnić ich żądanie w ciągu miesiąca. Gdy przetwarzanie jest ograniczone, możesz nadal przechowywać ich dane. Musisz powiadomić osobę, zanim ponownie rozpoczniesz przetwarzanie jej danych.</t>
+  </si>
+  <si>
+    <t>Oznacza to, że powinieneś być w stanie przesłać ich dane osobowe (Artykuł 20) w powszechnie czytelnym formacie (np. arkusz kalkulacyjny) do nich lub do wyznaczonej przez nich strony trzeciej. Może to wydawać się niesprawiedliwe z biznesowego punktu widzenia, ponieważ możesz być zmuszony przekazać dane swoich klientów konkurencji. Jednak z punktu widzenia prywatności, idea jest taka, że ludzie są właścicielami swoich danych, a nie Ty.</t>
+  </si>
+  <si>
+    <t>Jeśli przetwarzasz ich dane w celach marketingu bezpośredniego, musisz natychmiast zaprzestać ich przetwarzania (Artykuł 21) w tym celu. W przeciwnym razie możesz być w stanie zakwestionować ich sprzeciw, jeśli możesz wykazać "przekonujące uzasadnione podstawy".</t>
+  </si>
+  <si>
+    <t>Niektóre organizacje używają zautomatyzowanych procesów (Artykuł 22) do podejmowania decyzji o ludziach, które mają skutki prawne lub "podobnie znaczące". Jeśli uważasz, że to dotyczy Ciebie, musisz ustanowić procedurę zapewniającą ochronę ich praw, wolności i uzasadnionych interesów. Musisz umożliwić osobom łatwe zgłaszanie interwencji człowieka, udział w decyzjach i kwestionowanie już podjętych decyzji.</t>
+  </si>
+  <si>
+    <t>Podpisz umowę o przetwarzanie danych między Twoją organizacją a wszelkimi stronami trzecimi, które przetwarzają dane osobowe w Twoim imieniu.</t>
+  </si>
+  <si>
+    <t>Jeśli Twoja organizacja znajduje się poza UE, wyznacz przedstawiciela w jednym z państw członkowskich UE.</t>
+  </si>
+  <si>
+    <t>Jeśli przetwarzasz dane dotyczące osób w konkretnym państwie członkowskim, musisz wyznaczyć przedstawiciela w tym kraju, który będzie komunikować się w Twoim imieniu z organami ochrony danych. RODO i jego oficjalne dokumenty wspierające nie dostarczają wskazówek dotyczących sytuacji, w których przetwarzanie dotyczy osób z UE w wielu państwach członkowskich. Dopóki ten wymóg nie zostanie zinterpretowany, warto wyznaczyć przedstawiciela w państwie członkowskim, które używa Twojego języka. Niektóre organizacje, jak organy publiczne, nie muszą wyznaczać przedstawiciela w UE.</t>
+  </si>
+  <si>
+    <t>Wyznacz Inspektora Ochrony Danych (jeśli to konieczne).</t>
+  </si>
+  <si>
+    <t>Są trzy sytuacje, w których organizacje muszą mieć Inspektora Ochrony Danych (IOD), ale warto mieć go nawet jeśli nie jest to wymagane. IOD powinien być ekspertem w zakresie ochrony danych, którego zadaniem jest monitorowanie zgodności z RODO, ocena ryzyk związanych z ochroną danych, doradztwo w zakresie ocen skutków dla ochrony danych i współpraca z regulatorami.</t>
+  </si>
+  <si>
+    <t>Twoim klientom łatwo jest zażądać i otrzymać wszystkie informacje, które masz na ich temat.</t>
+  </si>
+  <si>
+    <t>Osoby mają prawo wglądu do swoich danych osobowych (Artykuł 15) i sposobu ich wykorzystania. Mają też prawo wiedzieć, jak długo planujesz przechowywać ich informacje i dlaczego. Musisz wysłać im pierwszą kopię tych informacji za darmo, ale możesz pobrać rozsądną opłatę za kolejne kopie. Upewnij się, że możesz zweryfikować tożsamość osoby składającej wniosek. Powinieneś być w stanie zrealizować takie wnioski w ciągu miesiąca.</t>
+  </si>
+  <si>
+    <t>Twoim klientom łatwo jest poprawić lub zaktualizować nieścisłe lub niekompletne informacje.</t>
+  </si>
+  <si>
+    <t>Twoim klientom łatwo jest zażądać usunięcia swoich danych osobowych.</t>
+  </si>
+  <si>
+    <t>Twoim klientom łatwo jest zażądać zaprzestania przetwarzania ich danych.</t>
+  </si>
+  <si>
+    <t>Twoim klientom łatwo jest otrzymać kopię swoich danych osobowych w formacie, który można łatwo przekazać innej firmie.</t>
+  </si>
+  <si>
+    <t>Twoim klientom łatwo jest sprzeciwić się przetwarzaniu ich danych.</t>
+  </si>
+  <si>
+    <t>Jeśli podejmujesz decyzje o ludziach na podstawie zautomatyzowanych procesów, masz procedurę ochrony ich praw.</t>
+  </si>
+  <si>
+    <t>Organizacje, które zatrudniają co najmniej 250 pracowników lub przetwarzają dane o wysokim ryzyku, są zobowiązane do prowadzenia aktualnej i szczegółowej listy swoich czynności przetwarzania (art. 30 RODO) oraz muszą być przygotowane do przedstawienia tej listy organom nadzorczym na żądanie. Najlepszym sposobem na wykazanie zgodności z RODO jest stosowanie oceny skutków dla ochrony danych (art. 35 RODO). Organizacje zatrudniające mniej niż 250 pracowników również powinny przeprowadzić taką ocenę, co ułatwi spełnienie pozostałych wymagań RODO. W swojej liście powinieneś uwzględnić: cele przetwarzania, rodzaj przetwarzanych danych, kto ma do nich dostęp w organizacji, wszelkie strony trzecie mające dostęp (i ich lokalizację), co robisz, aby chronić dane (np. szyfrowanie) oraz kiedy planujesz je usunąć (o ile to możliwe).</t>
+  </si>
+  <si>
+    <t>Musisz przestrzegać zasad 'ochrony danych od samego projektowania i domyślnej ochrony danych' (privacy by design and by default), włączając w to wdrażanie 'odpowiednich środków technicznych i organizacyjnych' w celu ochrony danych. Innymi słowy, ochrona danych to coś, co teraz musisz uwzględniać za każdym razem, gdy robisz cokolwiek z danymi osobowymi innych osób. Musisz również upewnić się, że każde przetwarzanie danych osobowych jest zgodne z zasadami ochrony danych opisanymi w art. 5 RODO. Środki techniczne obejmują szyfrowanie, a środki organizacyjne to takie działania, jak ograniczanie ilości zbieranych danych osobowych lub usuwanie danych, których już nie potrzebujesz. Punkt polega na tym, aby to była kwestia, o której ty i twoi pracownicy zawsze pamiętali.</t>
+  </si>
+  <si>
+    <t>Większość narzędzi produkcyjnych używanych przez firmy jest obecnie dostępna z wbudowanym szyfrowaniem end-to-end, w tym poczta e-mail, komunikatory, notatki i przechowywanie w chmurze. RODO wymaga od organizacji stosowania szyfrowania lub pseudonimizacji, ilekroć jest to wykonalne.</t>
+  </si>
+  <si>
+    <t>Nawet jeśli twoje bezpieczeństwo techniczne jest silne, bezpieczeństwo operacyjne może nadal stanowić słaby punkt. Stwórz politykę bezpieczeństwa, która zapewni, że twoi członkowie zespołu są świadomi bezpieczeństwa danych. Powinna zawierać wskazówki dotyczące bezpieczeństwa poczty elektronicznej, haseł, uwierzytelniania dwuskładnikowego, szyfrowania urządzeń i VPN-ów. Pracownicy, którzy mają dostęp do danych osobowych i pracownicy nietechniczni, powinni otrzymać dodatkowe szkolenie z wymagań RODO.</t>
+  </si>
+  <si>
+    <t>Ocena wpływu na ochronę danych (także znana jako ocena wpływu na prywatność) to sposób, aby zrozumieć, jak twój produkt lub usługa mogą zagrozić danym twoich klientów, a także jak zminimalizować te ryzyka. Urząd Ochrony Danych Osobowych w Polsce ma na swojej stronie internetowej listę kontrolną oceny wpływu na ochronę danych. RODO wymaga od organizacji przeprowadzania tego rodzaju analizy, ilekroć planują używać danych ludzi w sposób, który jest 'prawdopodobnie ryzykowny dla ich praw i wolności'. Urząd zaleca przeprowadzanie jej za każdym razem, gdy zamierzasz przetwarzać dane osobowe.</t>
+  </si>
+  <si>
+    <t>Jeśli dojdzie do naruszenia bezpieczeństwa danych i dane osobowe zostaną ujawnione, jesteś zobowiązany do powiadomienia odpowiedniego organu nadzorczego w swojej jurysdykcji w ciągu 72 godzin. Lista wielu organów nadzorczych państw członkowskich UE jest dostępna tutaj. RODO nie określa, kogo powinieneś powiadomić, jeśli nie jesteś organizacją z siedzibą w UE. Dla osób w krajach anglojęzycznych spoza UE najłatwiej może być powiadomić Urząd Komisarza ds. Ochrony Danych w Irlandii. Również jesteś zobowiązany do szybkiego przekazania informacji o naruszeniu bezpieczeństwa osobom, których dane dotyczą, chyba że naruszenie jest mało prawdopodobne, aby je narazić na ryzyko (na przykład, jeśli skradzione dane są zaszyfrowane).</t>
+  </si>
+  <si>
+    <t>Innym aspektem 'ochrony danych od samego projektowania i domyślnej ochrony danych' (art. 25 RODO) jest zapewnienie, że w organizacji jest osoba odpowiedzialna za zgodność z RODO. Ta osoba powinna być upoważniona do oceny polityk ochrony danych i wdrażania tych polityk.</t>
+  </si>
+  <si>
+    <t>Lista kontrolna RODO dla administratorów danych</t>
+  </si>
+  <si>
+    <t>GDPR.EU Lista kontrolna RODO dla administratorów danych  (https://gdpr.eu/checklist/)</t>
+  </si>
+  <si>
+    <t>Liste de contrôle RGPD pour les responsables du traitement des données</t>
+  </si>
+  <si>
+    <t>Liste de contrôle RGPD pour les responsables du traitement des données  (https://gdpr.eu/checklist/)</t>
+  </si>
+  <si>
+    <t>Lista kontrolna RODO dla administratorów danych  (https://gdpr.eu/checklist/)</t>
+  </si>
+  <si>
+    <t>Base légale et transparence</t>
+  </si>
+  <si>
+    <t>Effectuez un audit d’information pour déterminer quelles informations vous traitez et qui y a accès.</t>
+  </si>
+  <si>
+    <t>Fournissez des informations claires sur le traitement de vos données et une justification légale dans votre politique de confidentialité.</t>
+  </si>
+  <si>
+    <t>Sécurité des données</t>
+  </si>
+  <si>
+    <t>Responsabilisation et gouvernance</t>
+  </si>
+  <si>
+    <t>Droits à la vie privée</t>
+  </si>
+  <si>
+    <t>Il est facile pour vos clients de demander et de recevoir toutes les informations que vous avez sur eux.</t>
+  </si>
+  <si>
+    <t>Il est facile pour vos clients de corriger ou de mettre à jour des informations inexactes ou incomplètes.</t>
+  </si>
+  <si>
+    <t>Il est facile pour vos clients de demander la suppression de leurs données personnelles.</t>
+  </si>
+  <si>
+    <t>Il est facile pour vos clients de vous demander d’arrêter de traiter leurs données.</t>
+  </si>
+  <si>
+    <t>Il est facile pour vos clients de recevoir une copie de leurs données personnelles dans un format qui peut être facilement transféré à une autre entreprise.</t>
+  </si>
+  <si>
+    <t>Il est facile pour vos clients de s’opposer à ce que vous traitiez leurs données.</t>
+  </si>
+  <si>
+    <t>Si vous prenez des décisions concernant des personnes sur la base de processus automatisés, vous disposez d’une procédure pour protéger leurs droits.</t>
+  </si>
+  <si>
+    <t>Disposez d’une justification légale de vos activités de traitement des données.</t>
+  </si>
+  <si>
+    <t>Prenez en compte la protection des données à tout moment, depuis le début du développement d’un produit jusqu’à chaque traitement de données.</t>
+  </si>
+  <si>
+    <t>Créez une politique de sécurité interne pour les membres de votre équipe et sensibilisez-les à la protection des données.</t>
+  </si>
+  <si>
+    <t>Sachez quand effectuer une analyse d’impact relative à la protection des données et mettez en place un processus pour la réaliser.</t>
+  </si>
+  <si>
+    <t>Mettez en place un processus pour informer les autorités et vos personnes concernées en cas de violation de données.</t>
+  </si>
+  <si>
+    <t>Désignez une personne chargée d’assurer la conformité au RGPD dans l’ensemble de votre organisation.</t>
+  </si>
+  <si>
+    <t>Signez un accord de traitement des données entre votre organisation et tout tiers qui traite des données personnelles en votre nom.</t>
+  </si>
+  <si>
+    <t>Si votre organisation se trouve en dehors de l’UE, désignez un représentant dans l’un des États membres de l’UE.</t>
+  </si>
+  <si>
+    <t>Nommez un délégué à la protection des données (si nécessaire)</t>
+  </si>
+  <si>
+    <t>Les organisations qui comptent au moins 250 employés ou qui effectuent des traitements de données à haut risque sont tenues de tenir à jour une liste détaillée de leurs activités de traitement (article 30) et d’être prêtes à montrer cette liste aux régulateurs sur demande. La meilleure façon de démontrer la conformité au RGPD est d’utiliser une analyse d’impact sur la protection des données (article 35).
+Les organisations de moins de 250 employés devraient également effectuer une évaluation, car cela facilitera la conformité aux autres exigences du RGPD. Dans votre liste, vous devez inclure : les finalités du traitement, le type de données que vous traitez, qui y a accès dans votre organisation, les tiers (et où ils se trouvent) qui y ont accès, ce que vous faites pour protéger les données (par exemple, le cryptage) et quand vous prévoyez de les effacer (si possible).</t>
+  </si>
+  <si>
+    <t>Le traitement des données est illégal au regard du RGPD à moins que vous ne puissiez le justifier selon l’une des six conditions énumérées à l’article 6. Les articles 7 à 11 contiennent d’autres dispositions relatives aux enfants et à des catégories particulières de données à caractère personnel. Examinez ces dispositions, choisissez une base légale pour le traitement et documentez votre justification. Notez que si vous choisissez le « consentement » comme base légale, il existe des obligations supplémentaires, notamment la possibilité de révoquer leur consentement en permanence. Si vous vous fondez sur la légalité des « intérêts légitimes », vous devez être en mesure de démontrer que vous avez effectué une évaluation des facteurs relatifs à la vie privée.</t>
+  </si>
+  <si>
+    <t>Vous devez dire aux gens que vous collectez leurs données et pourquoi (article 12). Vous devez expliquer comment les données sont traitées, qui y a accès et comment vous les protégez. Ces informations doivent être incluses dans votre politique de confidentialité et fournies aux personnes concernées au moment où vous collectez leurs données. Il doit être présenté « sous une forme concise, transparente, intelligible et facilement accessible, dans un langage clair et simple, notamment pour toute information s’adressant spécifiquement à un enfant ».</t>
+  </si>
+  <si>
+    <t>Vous devez suivre les principes de « protection des données dès la conception et par défaut », y compris la mise en œuvre de « mesures techniques et organisationnelles appropriées » pour protéger les données. En d’autres termes, la protection des données est quelque chose que vous devez désormais prendre en compte chaque fois que vous faites quoi que ce soit avec les données personnelles d’autres personnes. Vous devez également vous assurer que tout traitement de données à caractère personnel respecte les principes de protection des données décrits à l’article 5. Les mesures techniques comprennent le cryptage, et les mesures organisationnelles consistent à limiter la quantité de données personnelles que vous collectez ou à supprimer les données dont vous n’avez plus besoin. Le fait est que vous et vos employés devez en être toujours conscients.</t>
+  </si>
+  <si>
+    <t>La plupart des outils de productivité utilisés par les entreprises sont désormais disponibles avec un chiffrement de bout en bout intégré, notamment les e-mails, la messagerie, les notes et le stockage dans le cloud. Le RGPD exige que les organisations utilisent le cryptage ou la pseudeonymisation chaque fois que cela est possible.</t>
+  </si>
+  <si>
+    <t>Chiffrez, pseudonymisez ou anonymisez les données personnelles dans la mesure du possible.</t>
+  </si>
+  <si>
+    <t>Même si votre sécurité technique est forte, la sécurité opérationnelle peut toujours être un maillon faible. Créez une politique de sécurité qui garantit que les membres de votre équipe sont bien informés sur la sécurité des données. Il doit inclure des conseils sur la sécurité des e-mails, les mots de passe, l’authentification à deux facteurs, le cryptage des appareils et les VPN. Les employés qui ont accès aux données personnelles et les employés non techniques doivent recevoir une formation supplémentaire sur les exigences du RGPD.</t>
+  </si>
+  <si>
+    <t>Une analyse d’impact sur la protection des données (également appelée évaluation de l’impact sur la vie privée) est un moyen de vous aider à comprendre comment votre produit ou service pourrait mettre en péril les données de vos clients, ainsi que comment minimiser ces risques. L’Information Commissioner’s Office (ICO) du Royaume-Uni a publié une liste de contrôle d’évaluation de l’impact sur la protection des données sur son site Web. Le RGPD exige que les organisations effectuent ce type d’analyse chaque fois qu’elles prévoient d’utiliser les données des personnes de manière à ce qu’il soit « susceptible d’entraîner un risque élevé pour [leurs] droits et libertés ». L’ICO recommande de le faire à tout moment lorsque vous êtes sur le point de traiter des données personnelles.</t>
+  </si>
+  <si>
+    <t>En cas de violation de données et d’exposition de données personnelles, vous devez en informer l’autorité de contrôle de votre juridiction dans les 72 heures. Une liste de nombreuses autorités de surveillance des États membres de l’UE peut être consultée ici. Le RGPD ne précise pas qui vous devez notifier si vous n’êtes pas une organisation basée dans l’UE. Pour ceux qui se trouvent dans des pays anglophones non membres de l’UE, il peut être plus facile d’en informer le Bureau du commissaire à la protection des données en Irlande. Vous êtes également tenu de communiquer rapidement les violations de données à vos personnes concernées, sauf si la violation n’est pas susceptible de les mettre en danger (par exemple, si les données volées sont cryptées).</t>
+  </si>
+  <si>
+    <t>Une autre partie de la « protection des données dès la conception et par défaut » (article 25) consiste à s’assurer qu’une personne de votre organisation est responsable de la conformité au RGPD. Cette personne devrait être habilitée à évaluer les politiques de protection des données et la mise en œuvre de ces politiques.</t>
+  </si>
+  <si>
+    <t>Cela inclut tous les services tiers qui traitent les données personnelles de vos personnes concernées, y compris les logiciels analytiques, les services de messagerie, les serveurs cloud, etc. La grande majorité des services ont un accord standard de traitement des données disponible sur leurs sites Web pour que vous puissiez les consulter. Ils énoncent les droits et obligations de chaque partie en matière de conformité au RGPD. Vous ne devez faire appel qu’à des tiers fiables et capables d’apporter des garanties suffisantes en matière de protection des données.</t>
+  </si>
+  <si>
+    <t>Si vous traitez des données relatives à des personnes dans un État membre particulier, vous devez désigner un représentant dans ce pays qui peut communiquer en votre nom avec les autorités de protection des données. Le RGPD et ses documents officiels ne donnent pas d’indications pour les situations où le traitement affecte des personnes de l’UE dans plusieurs États membres. Jusqu’à ce que cette exigence soit interprétée, il peut être prudent de désigner un représentant dans un État membre qui utilise votre langue. Certaines organisations, comme les organismes publics, ne sont pas tenues de désigner un représentant dans l’UE.</t>
+  </si>
+  <si>
+    <t>Il existe trois circonstances dans lesquelles les organisations sont tenues d’avoir un délégué à la protection des données (DPO), mais ce n’est pas une mauvaise idée d’en avoir un même si la règle ne s’applique pas à vous. Le DPD doit être un expert en matière de protection des données dont le travail consiste à surveiller la conformité au RGPD, à évaluer les risques liés à la protection des données, à donner des conseils sur les analyses d’impact relatives à la protection des données et à coopérer avec les régulateurs.</t>
+  </si>
+  <si>
+    <t>Les gens ont le droit de voir quelles données personnelles vous détenez à leur sujet (article 15) et comment vous les utilisez. Ils ont également le droit de savoir combien de temps vous prévoyez de conserver leurs informations et la raison pour laquelle elles sont conservées pendant cette période. Vous devez leur envoyer la première copie de ces informations gratuitement, mais vous pouvez facturer des frais raisonnables pour les copies suivantes. Assurez-vous de pouvoir vérifier l’identité de la personne qui demande les données. Vous devriez être en mesure de donner suite à ces demandes dans un délai d’un mois.</t>
+  </si>
+  <si>
+    <t>Faites de votre mieux pour maintenir les données à jour en mettant en place un processus de qualité des données, et faites en sorte qu’il soit facile pour vos clients de consulter (Article 15) et de mettre à jour leurs informations personnelles pour en assurer l’exactitude et l’exhaustivité. Assurez-vous de pouvoir vérifier l’identité de la personne qui demande les données. Vous devriez être en mesure de donner suite aux demandes au titre de l’article 16 dans un délai d’un mois.</t>
+  </si>
+  <si>
+    <t>Les gens ont généralement le droit de vous demander de supprimer toutes les données personnelles que vous avez à leur sujet, et vous devez honorer leur demande dans un délai d’environ un mois. Il y a cinq motifs pour lesquels vous pouvez refuser la demande, tels que l’exercice de la liberté d’expression ou le respect d’une obligation légale. Vous devez également tenter de vérifier l’identité de la personne qui fait la demande.</t>
+  </si>
+  <si>
+    <t>Vos personnes concernées peuvent demander à restreindre ou à arrêter le traitement de leurs données (article 18) si certains motifs s’appliquent, principalement en cas de litige quant à la licéité du traitement ou à l’exactitude des données. Vous êtes tenu d’honorer leur demande dans un délai d’environ un mois. Bien que le traitement soit limité, vous êtes toujours autorisé à continuer à stocker leurs données. Vous devez informer la personne concernée avant de recommencer à traiter ses données.</t>
+  </si>
+  <si>
+    <t>Cela signifie que vous devez être en mesure d’envoyer leurs données personnelles (article 20) dans un format lisible par tous (par exemple une feuille de calcul) soit à eux, soit à un tiers qu’ils désignent. Cela peut sembler injuste d’un point de vue commercial, dans la mesure où vous devrez peut-être remettre les données de vos clients à un concurrent. Mais du point de vue de la protection de la vie privée, l’idée est que ce sont les gens qui sont propriétaires de leurs données, pas vous.</t>
+  </si>
+  <si>
+    <t>Si vous traitez leurs données à des fins de marketing direct, vous devez cesser immédiatement de les traiter (article 21) à cette fin. Sinon, vous pourrez peut-être contester leur objection si vous pouvez démontrer l’existence de « motifs légitimes impérieux ».</t>
+  </si>
+  <si>
+    <t>Certains types d’organisations utilisent des processus automatisés (article 22) pour les aider à prendre des décisions concernant des personnes qui ont des effets juridiques ou « d’importance similaire ». Si vous pensez que cela s’applique à vous, vous devrez mettre en place une procédure pour vous assurer que vous protégez leurs droits, libertés et intérêts légitimes. Vous devez permettre aux gens de demander facilement une intervention humaine, de peser sur les décisions et de remettre en question les décisions que vous avez déjà prises.</t>
+  </si>
+  <si>
+    <t>library_name[pl]</t>
+  </si>
+  <si>
+    <t>library_description[pl]</t>
+  </si>
+  <si>
+    <t>framework_name[pl]</t>
+  </si>
+  <si>
+    <t>framework_description[pl]</t>
+  </si>
+  <si>
+    <t>name[pl]</t>
+  </si>
+  <si>
+    <t>description[pl]</t>
+  </si>
+  <si>
+    <t>library_name[fr]</t>
+  </si>
+  <si>
+    <t>library_description[fr]</t>
+  </si>
+  <si>
+    <t>framework_name[fr]</t>
+  </si>
+  <si>
+    <t>framework_description[fr]</t>
+  </si>
+  <si>
+    <t>name[fr]</t>
+  </si>
+  <si>
+    <t>description[fr]</t>
   </si>
 </sst>
 </file>
@@ -655,15 +959,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF7573E-4E40-7F4B-9C11-18EBEFA31BD0}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A8" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="130.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -680,7 +984,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -780,6 +1084,70 @@
       </c>
       <c r="C14" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -789,19 +1157,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD55C02-9331-C44C-8CCF-2A38E6CFDE74}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="66.1640625" customWidth="1"/>
+    <col min="6" max="6" width="54.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="91.83203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="47.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -811,50 +1182,92 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="289" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -867,16 +1280,34 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -889,8 +1320,20 @@
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -903,8 +1346,20 @@
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="F8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -917,8 +1372,20 @@
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -931,8 +1398,20 @@
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -945,16 +1424,34 @@
       <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -967,8 +1464,20 @@
       <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -981,8 +1490,20 @@
       <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -995,38 +1516,86 @@
       <c r="E15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
+      <c r="F16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1034,13 +1603,25 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1048,13 +1629,25 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1062,13 +1655,25 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1076,13 +1681,25 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1090,13 +1707,25 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1104,24 +1733,22 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>